<commit_message>
Auto-committed on 2022/12/12 週一 11:44:01.08
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L5-管理性作業/NegAppr01.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L5-管理性作業/NegAppr01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\DB\GenTables\L5-管理性作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9747F6C-66D1-475F-B108-F6B7D491A255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2780C435-0B39-42F9-972B-9BFBA565E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="111">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -437,6 +437,22 @@
   </si>
   <si>
     <t>BatchTxtNo = , AND RemitBank = , AND ApprDate=</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExportDate= , AND FinCode=</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExportDate DESC ,CustNo ASC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustNo ASC</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>findExporFinCode</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -652,7 +668,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -668,10 +684,10 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -683,9 +699,6 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -698,9 +711,6 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,7 +726,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -725,10 +735,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,9 +761,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1116,26 +1120,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="6" style="16" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="18" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.77734375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="16" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="14" customWidth="1"/>
     <col min="8" max="16384" width="21.44140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
@@ -1147,78 +1151,78 @@
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="32.4">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" s="15" customFormat="1">
+      <c r="D7" s="12"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="8" t="s">
         <v>0</v>
       </c>
@@ -1237,455 +1241,455 @@
       <c r="F8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="19">
+      <c r="A9" s="17">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="28">
         <v>8</v>
       </c>
-      <c r="F9" s="31"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="19">
+      <c r="A10" s="17">
         <v>2</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="28">
         <v>6</v>
       </c>
-      <c r="F10" s="31"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="19">
+      <c r="A11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="28">
         <v>8</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="19">
+      <c r="A12" s="17">
         <v>4</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="29">
         <v>10</v>
       </c>
-      <c r="F12" s="33"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="19">
+      <c r="A13" s="17">
         <v>5</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="29">
         <v>7</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="25" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="19">
+      <c r="A14" s="17">
         <v>6</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="29">
         <v>3</v>
       </c>
-      <c r="F14" s="31"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:7" ht="81">
-      <c r="A15" s="19">
+      <c r="A15" s="17">
         <v>7</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="29">
         <v>1</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="29" t="s">
+      <c r="F15" s="28"/>
+      <c r="G15" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="19">
+      <c r="A16" s="17">
         <v>8</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="28">
         <v>16</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>9</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="28">
         <v>16</v>
       </c>
-      <c r="F17" s="31">
+      <c r="F17" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="19">
+      <c r="A18" s="17">
         <v>10</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="29">
         <v>5</v>
       </c>
-      <c r="F18" s="31">
+      <c r="F18" s="28">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="19">
+      <c r="A19" s="17">
         <v>11</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="28">
         <v>8</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="30" t="s">
+      <c r="F19" s="28"/>
+      <c r="G19" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="19">
+      <c r="A20" s="17">
         <v>12</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="28">
         <v>8</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="30" t="s">
+      <c r="F20" s="28"/>
+      <c r="G20" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="19">
+      <c r="A21" s="17">
         <v>13</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="28">
         <v>8</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="30" t="s">
+      <c r="F21" s="28"/>
+      <c r="G21" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="19">
+      <c r="A22" s="17">
         <v>14</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="29">
         <v>7</v>
       </c>
-      <c r="F22" s="31"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="19">
+      <c r="A23" s="17">
         <v>15</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="28">
         <v>16</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="19">
+      <c r="A24" s="17">
         <v>16</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="28">
         <v>8</v>
       </c>
-      <c r="F24" s="31"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="19">
+      <c r="A25" s="17">
         <v>17</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="29">
         <v>8</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="30" t="s">
+      <c r="F25" s="28"/>
+      <c r="G25" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="19">
+      <c r="A26" s="17">
         <v>18</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="28">
         <v>4</v>
       </c>
-      <c r="F26" s="31"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="19">
+      <c r="A27" s="17">
         <v>19</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="28">
         <v>10</v>
       </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="30" t="s">
+      <c r="F27" s="28"/>
+      <c r="G27" s="27" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="19">
+      <c r="A28" s="17">
         <v>20</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="31"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="19">
+      <c r="A29" s="17">
         <v>21</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="25">
         <v>6</v>
       </c>
-      <c r="F29" s="33"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="19">
+      <c r="A30" s="17">
         <v>22</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="33"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="19">
+      <c r="A31" s="17">
         <v>23</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="28">
+      <c r="E31" s="25">
         <v>6</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="F32" s="33"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="6:6">
-      <c r="F33" s="33"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="6:6">
-      <c r="F34" s="33"/>
+      <c r="F34" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1705,11 +1709,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -1739,7 +1743,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1787,7 +1791,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="18" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1833,8 +1837,19 @@
       <c r="B12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="1" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>